<commit_message>
Test result of 9 participants and updated script
</commit_message>
<xml_diff>
--- a/experimental study/Evaluation sentences.xlsx
+++ b/experimental study/Evaluation sentences.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39327\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39327\Documents\GitHub\ConstitutionalGuardians\experimental study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B0D8CF-5AC7-4545-BE35-030D9C09946A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB07AD02-3095-4D2E-94F6-6C5B4D53C8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E376BB4-2300-418F-8364-2D231402B3BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>instruction</t>
   </si>
@@ -192,6 +192,27 @@
   </si>
   <si>
     <t>s_Disapproval.wav</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>think</t>
+  </si>
+  <si>
+    <t>angry</t>
+  </si>
+  <si>
+    <t>concerned</t>
+  </si>
+  <si>
+    <t>listen / admire</t>
+  </si>
+  <si>
+    <t>suspicious / terror / oops</t>
   </si>
 </sst>
 </file>
@@ -338,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -346,37 +367,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -384,6 +390,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,72 +427,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1A36554-58C6-2D42-B4A2-470AE8D0AC00}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6355080" y="4754880"/>
-          <a:ext cx="4351020" cy="1546860"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75283B9B-A6CC-434E-9C9D-2AAB7EDD9837}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="120" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="133.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -855,7 +816,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="93.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -884,7 +845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="67.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -915,120 +876,109 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="D13" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>51</v>
+      <c r="D14" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1039,6 +989,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>